<commit_message>
Updated with new day filter 3
</commit_message>
<xml_diff>
--- a/schedule_october_all.xlsx
+++ b/schedule_october_all.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E201"/>
+  <dimension ref="A1:E225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,12 +463,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hau Trung Hieu</t>
+          <t>Vu Ngoc Son</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -490,12 +490,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Dang Tien Dat</t>
+          <t>Ma Dinh Hung</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -517,12 +517,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Nguyen Hong Anh</t>
+          <t>Nguyen Thi Dinh</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -544,12 +544,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Vu Ngoc Son</t>
+          <t>Hoang Quoc Cuong</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -571,12 +571,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Pham Thi Ngoc Anh</t>
+          <t>Trieu Trung Kien</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -598,12 +598,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Tung</t>
+          <t>Tran Duc Hai</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -625,12 +625,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Nguyen Thi Thuy</t>
+          <t>Duong Thi Huong</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -652,12 +652,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Trieu Duc Manh</t>
+          <t>Trieu Linh Chi</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -679,12 +679,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Nguyen Hong Anh</t>
+          <t>Nguyen Ngoc Tung</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -706,7 +706,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -733,12 +733,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Dang Tuan Anh</t>
+          <t>Hau Trung Hieu</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -760,12 +760,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Hoang Hai Khang</t>
+          <t>Trieu Linh Chi</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -787,12 +787,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Nguyen Thi Dinh</t>
+          <t>Nguyen Ngoc Son</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -814,12 +814,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Dang Tien Dat</t>
+          <t>Pham Thi Ngoc Huyen</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -841,12 +841,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Hau Trung Hieu</t>
+          <t>Nguyen Ngoc Giao</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -868,12 +868,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Gia Phong</t>
+          <t>Trieu Duc Manh</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -895,12 +895,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Pham Thi Ngoc Huyen</t>
+          <t>Hoang Quoc Cuong</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -922,12 +922,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Tran Duc Hai</t>
+          <t>Dang Tien Dat</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -949,12 +949,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Dao Ngoc Trang</t>
+          <t>Dang Tuan Anh</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -976,12 +976,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Duong Thi Huong</t>
+          <t>Nguyen Thi Dinh</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1003,7 +1003,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1030,12 +1030,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Hoang Quoc Cuong</t>
+          <t>Nguyen Ngoc Long</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1057,12 +1057,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Trieu Duc Manh</t>
+          <t>Gia Phong</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1084,12 +1084,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Trieu Linh Chi</t>
+          <t>Duong Thi Huong</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1111,12 +1111,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Giao</t>
+          <t>Trieu Trung Kien</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1138,12 +1138,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Do Thi Hue</t>
+          <t>Dao Ngoc Trang</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1165,12 +1165,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Ma Dinh Hung</t>
+          <t>Hoang Hai Khang</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1192,12 +1192,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Trieu Trung Kien</t>
+          <t>Nguyen Hong Anh</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1219,12 +1219,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Luong Nguyen Thanh Ha</t>
+          <t>Ma Dinh Hung</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1246,7 +1246,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1273,12 +1273,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Son</t>
+          <t>Luong Nguyen Thanh Ha</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1300,12 +1300,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Tung</t>
+          <t>Tran Duc Hai</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1327,12 +1327,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Nguyen Thi Dinh</t>
+          <t>Nguyen Ngoc Giao</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1354,12 +1354,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Do Thi Hue</t>
+          <t>Luong Nguyen Thanh Ha</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1381,12 +1381,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Long</t>
+          <t>Nguyen Ngoc Son</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1408,12 +1408,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Hau Trung Hieu</t>
+          <t>Hoang Hai Khang</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1435,7 +1435,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1462,12 +1462,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Gia Phong</t>
+          <t>Nguyen Hong Anh</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1489,12 +1489,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Nguyen Van Trung</t>
+          <t>Pham Thi Ngoc Anh</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1516,12 +1516,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Trieu Trung Kien</t>
+          <t>Gia Phong</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1543,12 +1543,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Hoang Hai Khang</t>
+          <t>Trieu Linh Chi</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1570,12 +1570,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Nguyen Thi Thuy</t>
+          <t>Trieu Duc Manh</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1597,12 +1597,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Giao</t>
+          <t>Do Thi Hue</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1624,7 +1624,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1651,12 +1651,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Pham Thi Ngoc Anh</t>
+          <t>Pham Thi Ngoc Huyen</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1678,12 +1678,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Nguyen Hong Anh</t>
+          <t>Hoang Quoc Cuong</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1705,12 +1705,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Pham Thi Ngoc Huyen</t>
+          <t>Nguyen Thi Dinh</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1732,12 +1732,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Luong Nguyen Thanh Ha</t>
+          <t>Trieu Trung Kien</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1759,12 +1759,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Trieu Duc Manh</t>
+          <t>Duong Thi Huong</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1786,12 +1786,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Vu Ngoc Son</t>
+          <t>Ma Dinh Hung</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1813,12 +1813,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Tung</t>
+          <t>Nguyen Ngoc Long</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1840,12 +1840,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Duong Thi Huong</t>
+          <t>Hau Trung Hieu</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1867,12 +1867,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Trieu Linh Chi</t>
+          <t>Vu Ngoc Son</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1894,12 +1894,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Dang Tien Dat</t>
+          <t>Nguyen Thi Thuy</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1921,7 +1921,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1948,12 +1948,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Hoang Quoc Cuong</t>
+          <t>Nguyen Van Trung</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1975,12 +1975,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Hoang Quoc Cuong</t>
+          <t>Tran Duc Hai</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2002,12 +2002,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Pham Thi Ngoc Huyen</t>
+          <t>Do Thi Hue</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2029,12 +2029,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Nguyen Thi Dinh</t>
+          <t>Trieu Trung Kien</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2056,12 +2056,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Long</t>
+          <t>Nguyen Thi Dinh</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2083,12 +2083,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Giao</t>
+          <t>Nguyen Thi Thuy</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2110,12 +2110,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Nguyen Thi Thuy</t>
+          <t>Trieu Duc Manh</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2137,12 +2137,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Ma Dinh Hung</t>
+          <t>Duong Thi Huong</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2164,12 +2164,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Tung</t>
+          <t>Trieu Linh Chi</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2191,12 +2191,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Duong Thi Huong</t>
+          <t>Pham Thi Ngoc Huyen</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2218,12 +2218,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Trieu Trung Kien</t>
+          <t>Hau Trung Hieu</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2245,12 +2245,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Luong Nguyen Thanh Ha</t>
+          <t>Nguyen Hong Anh</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2272,12 +2272,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Dang Tuan Anh</t>
+          <t>Nguyen Ngoc Son</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2299,12 +2299,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Dang Tien Dat</t>
+          <t>Hoang Quoc Cuong</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2326,12 +2326,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Gia Phong</t>
+          <t>Luong Nguyen Thanh Ha</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2353,12 +2353,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Hoang Hai Khang</t>
+          <t>Vu Ngoc Son</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2380,12 +2380,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Do Thi Hue</t>
+          <t>Dang Tien Dat</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2407,12 +2407,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Pham Thi Ngoc Anh</t>
+          <t>Dang Tuan Anh</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2434,12 +2434,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Nguyen Van Trung</t>
+          <t>Hoang Hai Khang</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2461,12 +2461,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Son</t>
+          <t>Nguyen Ngoc Tung</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2488,12 +2488,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Tran Duc Hai</t>
+          <t>Gia Phong</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2515,12 +2515,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Vu Ngoc Son</t>
+          <t>Nguyen Van Trung</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2542,12 +2542,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Trieu Linh Chi</t>
+          <t>Ma Dinh Hung</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2569,12 +2569,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Nguyen Hong Anh</t>
+          <t>Nguyen Ngoc Giao</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2596,12 +2596,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-10-26</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Trieu Duc Manh</t>
+          <t>Dao Ngoc Trang</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2623,12 +2623,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Son</t>
+          <t>Nguyen Ngoc Tung</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2650,12 +2650,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Duong Thi Huong</t>
+          <t>Trieu Duc Manh</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2677,12 +2677,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Hau Trung Hieu</t>
+          <t>Pham Thi Ngoc Anh</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2704,12 +2704,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Trieu Linh Chi</t>
+          <t>Dao Ngoc Trang</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2731,12 +2731,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Dao Ngoc Trang</t>
+          <t>Nguyen Van Trung</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2758,12 +2758,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Dang Tuan Anh</t>
+          <t>Nguyen Hong Anh</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2785,12 +2785,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Nguyen Hong Anh</t>
+          <t>Ma Dinh Hung</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2812,12 +2812,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Hoang Quoc Cuong</t>
+          <t>Vu Ngoc Son</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2839,12 +2839,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Vu Ngoc Son</t>
+          <t>Nguyen Ngoc Giao</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2866,12 +2866,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Tung</t>
+          <t>Duong Thi Huong</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2893,12 +2893,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Pham Thi Ngoc Huyen</t>
+          <t>Tran Duc Hai</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2920,12 +2920,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Gia Phong</t>
+          <t>Trieu Trung Kien</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2947,12 +2947,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Tran Duc Hai</t>
+          <t>Nguyen Ngoc Son</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2974,12 +2974,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Luong Nguyen Thanh Ha</t>
+          <t>Hoang Hai Khang</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3001,12 +3001,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Nguyen Van Trung</t>
+          <t>Nguyen Ngoc Long</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3028,12 +3028,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Trieu Duc Manh</t>
+          <t>Nguyen Thi Thuy</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3055,12 +3055,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Dang Tien Dat</t>
+          <t>Hoang Quoc Cuong</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3082,12 +3082,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Do Thi Hue</t>
+          <t>Luong Nguyen Thanh Ha</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3109,12 +3109,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Long</t>
+          <t>Hau Trung Hieu</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3136,12 +3136,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Nguyen Thi Dinh</t>
+          <t>Dang Tuan Anh</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3163,12 +3163,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Trieu Trung Kien</t>
+          <t>Do Thi Hue</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3190,12 +3190,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Nguyen Thi Thuy</t>
+          <t>Dang Tien Dat</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3217,12 +3217,12 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Giao</t>
+          <t>Nguyen Thi Dinh</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3244,12 +3244,12 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-26</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Hoang Hai Khang</t>
+          <t>Pham Thi Ngoc Huyen</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3271,12 +3271,12 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Vu Ngoc Son</t>
+          <t>Pham Thi Ngoc Huyen</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3298,12 +3298,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Dang Tien Dat</t>
+          <t>Nguyen Hong Anh</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3325,12 +3325,12 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Ma Dinh Hung</t>
+          <t>Trieu Linh Chi</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3352,12 +3352,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Long</t>
+          <t>Dang Tuan Anh</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3379,12 +3379,12 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Trieu Duc Manh</t>
+          <t>Nguyen Ngoc Giao</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3406,12 +3406,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Nguyen Van Trung</t>
+          <t>Duong Thi Huong</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3433,12 +3433,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Dang Tuan Anh</t>
+          <t>Luong Nguyen Thanh Ha</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3460,12 +3460,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Nguyen Thi Thuy</t>
+          <t>Nguyen Thi Dinh</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3487,12 +3487,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Do Thi Hue</t>
+          <t>Dang Tien Dat</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3514,12 +3514,12 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Luong Nguyen Thanh Ha</t>
+          <t>Hoang Quoc Cuong</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3541,12 +3541,12 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Dao Ngoc Trang</t>
+          <t>Gia Phong</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3568,12 +3568,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Son</t>
+          <t>Hoang Hai Khang</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -3595,12 +3595,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Pham Thi Ngoc Anh</t>
+          <t>Nguyen Thi Thuy</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -3622,12 +3622,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Giao</t>
+          <t>Ma Dinh Hung</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -3649,12 +3649,12 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Trieu Trung Kien</t>
+          <t>Nguyen Ngoc Son</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -3676,12 +3676,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Pham Thi Ngoc Huyen</t>
+          <t>Tran Duc Hai</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -3703,12 +3703,12 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Gia Phong</t>
+          <t>Do Thi Hue</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -3730,12 +3730,12 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Hoang Quoc Cuong</t>
+          <t>Pham Thi Ngoc Anh</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -3757,12 +3757,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Nguyen Hong Anh</t>
+          <t>Dao Ngoc Trang</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -3784,12 +3784,12 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Tung</t>
+          <t>Nguyen Ngoc Long</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -3811,12 +3811,12 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Duong Thi Huong</t>
+          <t>Nguyen Van Trung</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -3838,12 +3838,12 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Hau Trung Hieu</t>
+          <t>Nguyen Ngoc Tung</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -3865,12 +3865,12 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Tran Duc Hai</t>
+          <t>Trieu Duc Manh</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -3892,12 +3892,12 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-27</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Hoang Hai Khang</t>
+          <t>Vu Ngoc Son</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -3919,12 +3919,12 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Gia Phong</t>
+          <t>Dang Tien Dat</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -3946,12 +3946,12 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Trieu Linh Chi</t>
+          <t>Ma Dinh Hung</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -3973,12 +3973,12 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Ma Dinh Hung</t>
+          <t>Nguyen Thi Dinh</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -4000,12 +4000,12 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Trieu Duc Manh</t>
+          <t>Nguyen Thi Thuy</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -4027,12 +4027,12 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Vu Ngoc Son</t>
+          <t>Duong Thi Huong</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -4054,12 +4054,12 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Son</t>
+          <t>Trieu Linh Chi</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4081,12 +4081,12 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Tran Duc Hai</t>
+          <t>Nguyen Ngoc Long</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -4108,12 +4108,12 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Trieu Trung Kien</t>
+          <t>Dao Ngoc Trang</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -4135,12 +4135,12 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Dang Tien Dat</t>
+          <t>Gia Phong</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -4162,12 +4162,12 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Hau Trung Hieu</t>
+          <t>Nguyen Ngoc Son</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -4189,12 +4189,12 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Nguyen Hong Anh</t>
+          <t>Hoang Quoc Cuong</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -4216,12 +4216,12 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Pham Thi Ngoc Anh</t>
+          <t>Hoang Hai Khang</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -4243,12 +4243,12 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Long</t>
+          <t>Hau Trung Hieu</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -4270,12 +4270,12 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Nguyen Thi Dinh</t>
+          <t>Tran Duc Hai</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -4297,12 +4297,12 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Dang Tuan Anh</t>
+          <t>Do Thi Hue</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -4324,12 +4324,12 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Dao Ngoc Trang</t>
+          <t>Dang Tuan Anh</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -4351,12 +4351,12 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Nguyen Thi Thuy</t>
+          <t>Nguyen Ngoc Giao</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -4378,12 +4378,12 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Do Thi Hue</t>
+          <t>Pham Thi Ngoc Huyen</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -4405,7 +4405,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4432,12 +4432,12 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Pham Thi Ngoc Huyen</t>
+          <t>Nguyen Van Trung</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -4459,12 +4459,12 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Hoang Hai Khang</t>
+          <t>Nguyen Ngoc Tung</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -4486,12 +4486,12 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Giao</t>
+          <t>Trieu Duc Manh</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -4513,12 +4513,12 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Nguyen Van Trung</t>
+          <t>Trieu Trung Kien</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -4540,12 +4540,12 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Duong Thi Huong</t>
+          <t>Vu Ngoc Son</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -4567,12 +4567,12 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Long</t>
+          <t>Nguyen Ngoc Son</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -4594,12 +4594,12 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Tung</t>
+          <t>Nguyen Thi Thuy</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -4621,12 +4621,12 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Pham Thi Ngoc Anh</t>
+          <t>Trieu Linh Chi</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -4648,7 +4648,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -4675,12 +4675,12 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Nguyen Thi Dinh</t>
+          <t>Nguyen Ngoc Long</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -4702,12 +4702,12 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Do Thi Hue</t>
+          <t>Pham Thi Ngoc Huyen</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -4729,12 +4729,12 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Gia Phong</t>
+          <t>Ma Dinh Hung</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -4756,12 +4756,12 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Nguyen Hong Anh</t>
+          <t>Nguyen Ngoc Tung</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -4783,12 +4783,12 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Hoang Hai Khang</t>
+          <t>Duong Thi Huong</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -4810,12 +4810,12 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Luong Nguyen Thanh Ha</t>
+          <t>Hau Trung Hieu</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -4837,12 +4837,12 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Nguyen Van Trung</t>
+          <t>Hoang Quoc Cuong</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -4864,12 +4864,12 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Trieu Trung Kien</t>
+          <t>Luong Nguyen Thanh Ha</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -4891,12 +4891,12 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Vu Ngoc Son</t>
+          <t>Trieu Duc Manh</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -4918,12 +4918,12 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Dang Tuan Anh</t>
+          <t>Do Thi Hue</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -4945,12 +4945,12 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Trieu Linh Chi</t>
+          <t>Vu Ngoc Son</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -4972,12 +4972,12 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Pham Thi Ngoc Huyen</t>
+          <t>Hoang Hai Khang</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -4999,12 +4999,12 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Hoang Quoc Cuong</t>
+          <t>Pham Thi Ngoc Anh</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -5026,12 +5026,12 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Hau Trung Hieu</t>
+          <t>Nguyen Ngoc Giao</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -5053,12 +5053,12 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Trieu Duc Manh</t>
+          <t>Dang Tuan Anh</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -5080,12 +5080,12 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Dao Ngoc Trang</t>
+          <t>Trieu Trung Kien</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -5107,12 +5107,12 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Nguyen Thi Thuy</t>
+          <t>Nguyen Thi Dinh</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -5134,12 +5134,12 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Giao</t>
+          <t>Nguyen Hong Anh</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -5161,12 +5161,12 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Dang Tien Dat</t>
+          <t>Dao Ngoc Trang</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -5188,12 +5188,12 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Son</t>
+          <t>Dang Tien Dat</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -5215,12 +5215,12 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Hau Trung Hieu</t>
+          <t>Dao Ngoc Trang</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -5242,12 +5242,12 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Nguyen Van Trung</t>
+          <t>Hoang Hai Khang</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -5269,12 +5269,12 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Dao Ngoc Trang</t>
+          <t>Nguyen Van Trung</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -5296,12 +5296,12 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Dang Tuan Anh</t>
+          <t>Nguyen Hong Anh</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -5323,12 +5323,12 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Tung</t>
+          <t>Do Thi Hue</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -5350,12 +5350,12 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Vu Ngoc Son</t>
+          <t>Trieu Linh Chi</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -5377,12 +5377,12 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Hoang Hai Khang</t>
+          <t>Nguyen Ngoc Long</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -5404,12 +5404,12 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Hoang Quoc Cuong</t>
+          <t>Pham Thi Ngoc Huyen</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -5431,12 +5431,12 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Long</t>
+          <t>Nguyen Ngoc Tung</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -5458,12 +5458,12 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Tran Duc Hai</t>
+          <t>Hoang Quoc Cuong</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -5485,12 +5485,12 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Pham Thi Ngoc Huyen</t>
+          <t>Ma Dinh Hung</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -5512,12 +5512,12 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Nguyen Ngoc Son</t>
+          <t>Luong Nguyen Thanh Ha</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -5539,12 +5539,12 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Nguyen Thi Thuy</t>
+          <t>Nguyen Ngoc Giao</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -5566,12 +5566,12 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Nguyen Hong Anh</t>
+          <t>Trieu Duc Manh</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
@@ -5593,12 +5593,12 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Trieu Linh Chi</t>
+          <t>Dang Tuan Anh</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -5620,12 +5620,12 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Do Thi Hue</t>
+          <t>Tran Duc Hai</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -5647,12 +5647,12 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Dang Tien Dat</t>
+          <t>Gia Phong</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -5674,12 +5674,12 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Ma Dinh Hung</t>
+          <t>Nguyen Thi Thuy</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -5701,12 +5701,12 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Pham Thi Ngoc Anh</t>
+          <t>Duong Thi Huong</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -5728,12 +5728,12 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Trieu Trung Kien</t>
+          <t>Vu Ngoc Son</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -5755,12 +5755,12 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Nguyen Thi Dinh</t>
+          <t>Dang Tien Dat</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -5782,12 +5782,12 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Trieu Duc Manh</t>
+          <t>Hau Trung Hieu</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -5809,12 +5809,12 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Duong Thi Huong</t>
+          <t>Nguyen Thi Dinh</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -5836,25 +5836,673 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
+          <t>2025-10-30</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Pham Thi Ngoc Anh</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>Shift 3</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
           <t>2025-10-31</t>
         </is>
       </c>
-      <c r="B201" t="inlineStr">
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Nguyen Thi Dinh</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>Shift 1</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Nguyen Hong Anh</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>Shift 1</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Tran Duc Hai</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>Shift 1</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Trieu Duc Manh</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>Shift 1</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Nguyen Ngoc Giao</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>Shift 1</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Dang Tien Dat</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>Shift 1</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Duong Thi Huong</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Shift 1</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Hau Trung Hieu</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>Shift 1</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Dang Tuan Anh</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>Shift 2</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Trieu Linh Chi</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Shift 2</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Vu Ngoc Son</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>Shift 2</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Nguyen Ngoc Tung</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>Shift 2</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Gia Phong</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>Shift 2</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Nguyen Thi Thuy</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>Shift 2</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Nguyen Ngoc Long</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>Shift 2</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Ma Dinh Hung</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>Shift 2</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
         <is>
           <t>Luong Nguyen Thanh Ha</t>
         </is>
       </c>
-      <c r="C201" t="inlineStr">
-        <is>
-          <t>Shift 3</t>
-        </is>
-      </c>
-      <c r="D201" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
-      <c r="E201" t="inlineStr">
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>Shift 3</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Pham Thi Ngoc Huyen</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>Shift 3</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Nguyen Ngoc Son</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>Shift 3</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Hoang Quoc Cuong</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>Shift 3</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Hoang Hai Khang</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>Shift 3</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Dao Ngoc Trang</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>Shift 3</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Do Thi Hue</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>Shift 3</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>23:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Nguyen Van Trung</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>Shift 3</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
         <is>
           <t>23:00</t>
         </is>

</xml_diff>